<commit_message>
Versão final de teste
</commit_message>
<xml_diff>
--- a/stims.xlsx
+++ b/stims.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A119"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,833 +436,1452 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>stimulus_time</t>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>stimulus</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dataset/httpabsolumentgratuitfreefrimagesbenaffleckjpg.jpg</t>
+          <t>Celebs/14_Emma_Watson_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dataset/httpafilesbiographycomimageuploadcfillcssrgbdprgfacehqwMTENDgMDUODczNDcNTcjpg.jpg</t>
+          <t>Celebs/14_Emma_Watson_0005.jpg</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dataset/httpafilesbiographycomimageuploadcfillcssrgbdprgfacehqwMTEODAOTcxNjcMjczMjkzjpg.jpg</t>
+          <t>Celebs/14_Emma_Watson_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dataset/httpafilesbiographycomimageuploadcfillcssrgbdprgfacehqwMTIOTcwODQNTUzNjQMzcjpg.jpg</t>
+          <t>Celebs/14_Emma_Watson_0013.jpg</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Dataset/httpafilesbiographycomimageuploadcfillcssrgbdprgfacehqwMTIwNjANjMMDINzIxNjcjpg.jpg</t>
+          <t>Celebs/14_Emma_Watson_0015.jpg</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dataset/httpassetsrollingstonecomassetsarticlemadonnadavidbowiechangedthecourseofmylifeforeversmallsquarexmadonnabowiejpg.jpg</t>
+          <t>Celebs/15_Margot_Robbie_0005.jpg</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Dataset/httpassetsrollingstonecomassetsimagesalbumreviewaffaceabdcccaeedjpg.jpg</t>
+          <t>Celebs/15_Margot_Robbie_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dataset/httpaurorasblogcomwpcontentuploadsjerryseinfeldpublicityshotjpg.jpg</t>
+          <t>Celebs/16_Emma_Stone_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Dataset/httpblognjcomentertainmentimpactcelebritiesmediumjerrybjpg.jpg</t>
+          <t>Celebs/16_Emma_Stone_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Dataset/httpbpblogspotcomedLMjVpRGkSWexgsXjkNIAAAAAAAADWgFFtAUqBlhAsjpg.jpg</t>
+          <t>Celebs/16_Emma_Stone_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dataset/httpcdncdnjustjaredcomwpcontentuploadsheadlineseltonjohnemmysperformancewatchnowjpg.jpg</t>
+          <t>Celebs/16_Emma_Stone_0014.jpg</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dataset/httpcdncdnjustjaredcomwpcontentuploadsheadlineseltonjohnstillstandingbrooklynnewyearsjpg.jpg</t>
+          <t>Celebs/16_Margot_Robbie_0009.jpg</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Dataset/httpcdncdnjustjaredcomwpcontentuploadsheadlineseltonjohnsupportsbrucejennerstransitiontowomanjpg.jpg</t>
+          <t>Celebs/17_Daniel_Radcliffe_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Dataset/httpcdncdnjustjaredcomwpcontentuploadsheadlinesjerryseinfeldmakesbrianwilliamsjokejpg.jpg</t>
+          <t>Celebs/17_Emma_Watson_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Dataset/httpcdncdnjustjaredcomwpcontentuploadsheadlinesmadonnatalksparisattackstearsjpg.jpg</t>
+          <t>Celebs/17_Margot_Robbie_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Dataset/httpcdncdnjustjaredcomwpcontentuploadsheadlinesmindykalingcomedypilotjpg.jpg</t>
+          <t>Celebs/17_Margot_Robbie_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Dataset/httpcdnfuncheapcomwpcontentuploadsVOGUEjpg.jpg</t>
+          <t>Celebs/17_Margot_Robbie_0014.jpg</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Dataset/httpcdnlyricssongonlyricsnetwpcontentuploadsEltonJohnDiscographyCDreleasesjpg.jpg</t>
+          <t>Celebs/18_Daniel_Radcliffe_0002.jpg</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dataset/httpcdnpastemagazinecomwwwarticlesmindykalingndbookjpg.jpg</t>
+          <t>Celebs/18_Daniel_Radcliffe_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dataset/httpcdnpastemagazinecomwwwarticlesmindyprojectjpg.jpg</t>
+          <t>Celebs/18_Daniel_Radcliffe_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dataset/httpcdnssninsidercomwpcontentuploadsjerryseinfeldxjpg.jpg</t>
+          <t>Celebs/18_Emma_Stone_0016.jpg</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Dataset/httpcsvkmeuaafdfjpg.jpg</t>
+          <t>Celebs/18_Emma_Watson_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Dataset/httpcsvkmeuadecafjpg.jpg</t>
+          <t>Celebs/19_Emma_Stone_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Dataset/httpcsvkmeuaeccjpg.jpg</t>
+          <t>Celebs/19_Margot_Robbie_0001.jpg</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Dataset/httpdbrbzkkbdsdcloudfrontnetwpcontentuploadsMindyKalingjpg.jpg</t>
+          <t>Celebs/19_Margot_Robbie_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Dataset/httpecximagesamazoncomimagesIfmaBKWLACULSRjpg.jpg</t>
+          <t>Celebs/20_Emma_Stone_0005.jpg</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Dataset/httpftqncomymusicLxZeltonjohnjpg.jpg</t>
+          <t>Celebs/20_Emma_Watson_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Dataset/httpgonetworthcomwpcontentuploadsthumbsjpg.jpg</t>
+          <t>Celebs/20_Margot_Robbie_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Dataset/httpgraphicsnytimescomimagesmagazinekalingkalingarticleInlinejpg.jpg</t>
+          <t>Celebs/20_Margot_Robbie_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Dataset/httpgraphicsnytimescomimagessectionmoviesfilmographyWireImagejpg.jpg</t>
+          <t>Celebs/20_Scarlett_Johansson_0011.jpg</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Dataset/httpiamediaimdbcomimagesMMVBMTANDQNTAxNDVeQTJeQWpwZBbWUMDIMjQOTYVUXCRALjpg.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0002.jpg</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Dataset/httpiamediaimdbcomimagesMMVBMTAxNDUMzUwOTdeQTJeQWpwZBbWUMDUOTAyNTIVUXCRALjpg.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Dataset/httpikinjaimgcomgawkermediaimageuploadsWmIuhdsrcedidjpgjpg.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0009.jpg</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Dataset/httpimagegaladevcmseamadonnaprivatdetektivsquaretopsquarejpgv.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Dataset/httpimagescontactmusiccomnewsimagesjerryseinfeldjpg.jpg</t>
+          <t>Celebs/21_Emma_Stone_0002.jpg</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Dataset/httpimagesfandangocomrImageRendererredesignstaticimgnoxportraitjpgpcpcpcimagesmasterrepositoryperformerimagespjpg.jpg</t>
+          <t>Celebs/21_Emma_Stone_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Dataset/httpimagesmtvcomurimgidfiledocrootvhcomsitewideflipbooksimgdailyjpgenlargefalsemattetruematteColorblackquality.jpg</t>
+          <t>Celebs/21_Emma_Watson_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Dataset/httpimagesnymagcomimagesdailymindykalingxjpg.jpg</t>
+          <t>Celebs/21_Margot_Robbie_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Dataset/httpimagesrottentomatoescomimagesspotlightsnewsjerryseinfeldjpg.jpg</t>
+          <t>Celebs/21_Scarlett_Johansson_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Dataset/httpimgclosermagfrvarclosermagstorageimagesactupeoplebiodestarsmadonnamadonnafreFRmadonnaexactxljpg.jpg</t>
+          <t>Celebs/22_Emma_Stone_0013.jpg</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Dataset/httpimggalpmdstaticnetfithttpAFFwwwEgalaEfrFvarFgalFstorageFimagesFmediaFmultiuploaddufevrierFeltonjohnFfreFRFeltonjohnEjpgxqualityeltonjohnjpg.jpg</t>
+          <t>Celebs/22_Emma_Watson_0001.jpg</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Dataset/httpimgthedrumcomsfspublicnewstmpjerryseinfeldjpg.jpg</t>
+          <t>Celebs/22_Emma_Watson_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Dataset/httpimgtimeincnetpeopleinewsjerryseinfeldjpg.jpg</t>
+          <t>Celebs/22_Emma_Watson_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Dataset/httpmediacacheecpinimgcomxffeffbcefjpg.jpg</t>
+          <t>Celebs/22_Margot_Robbie_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Dataset/httpmediaonsugarcomfilesbabaaaaaMindyInterviewxxxlargejpg.jpg</t>
+          <t>Celebs/22_Scarlett_Johansson_0005.jpg</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Dataset/httpmediapopsugarassetscomfilescbffewltonjpg.jpg</t>
+          <t>Celebs/23_Daniel_Radcliffe_0002.jpg</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Dataset/httpmediapopsugarassetscomfilesusersxlargejpg.jpg</t>
+          <t>Celebs/23_Daniel_Radcliffe_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Dataset/httpmediavoguecomrwblondesdarkbrowsmadonnajpg.jpg</t>
+          <t>Celebs/23_Daniel_Radcliffe_0019.jpg</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Dataset/httppfodcompchannelslegacyprofilejerryseinfeldpodcastjpg.jpg</t>
+          <t>Celebs/23_Emma_Stone_0014.jpg</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Dataset/httppixelnymagcomimgsfashiondailymindykalingwhjpg.jpg</t>
+          <t>Celebs/24_Daniel_Radcliffe_0017.jpg</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Dataset/httpresizeparismatchladmediafrrffffffcentermiddleimgvarnewsstorageimagesparismatchpeopleazmadonnafreFRMadonnajpg.jpg</t>
+          <t>Celebs/24_Emma_Stone_0015.jpg</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Dataset/httpsamazonawscomkidzworldphotoimagesbccdddaaadgallerymindykalinggalleryjpg.jpg</t>
+          <t>Celebs/24_Scarlett_Johansson_0001.jpg</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Dataset/httpsdfrpwlycscloudfrontnetdeltonjohnjpg.jpg</t>
+          <t>Celebs/24_Scarlett_Johansson_0011.jpg</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Dataset/httpsimagesnasslimagesamazoncomimagesIAQdwKvFILUXjpg.jpg</t>
+          <t>Celebs/25_Scarlett_Johansson_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Dataset/httpsimgbuzzfeedcombuzzfeedstaticstaticcampaignimageswebdradorableetsyitemsallmindykalingfansneedbigjpg.jpg</t>
+          <t>Celebs/26_Scarlett_Johansson_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Dataset/httpsmedialivenationcomartiststapjpg.jpg</t>
+          <t>Celebs/26_Scarlett_Johansson_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Dataset/httpspmctvlinefileswordpresscomeltonjohnjpg.jpg</t>
+          <t>Celebs/27_Scarlett_Johansson_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Dataset/httpsrobertaccetturacomwpcontentuploadsjerryseinfeldheadshotjpg.jpg</t>
+          <t>Celebs/28_Scarlett_Johansson_0005.jpg</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxaaeaaeecccaedfebdbjpg.jpg</t>
+          <t>Celebs/29_Scarlett_Johansson_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxafafedebcbjpg.jpg</t>
+          <t>Celebs/29_Scarlett_Johansson_0016.jpg</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxafaffbbbbdbcbdddjpg.jpg</t>
+          <t>Celebs/31_Neil_Patrick_Harris_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxbabafeacbaaacabffjpg.jpg</t>
+          <t>Celebs/32_Jim_Parsons_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxbbfcbdedfbfdbjpg.jpg</t>
+          <t>Celebs/32_Jim_Parsons_0016.jpg</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxcccccddbbfedabjpg.jpg</t>
+          <t>Celebs/32_Jim_Parsons_0018.jpg</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxccccdabeaadjpg.jpg</t>
+          <t>Celebs/33_Jim_Parsons_0011.jpg</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxdbbdbbbececacdecdcdfjpg.jpg</t>
+          <t>Celebs/33_Neil_Patrick_Harris_0011.jpg</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxdcfdcfedfaedadjpg.jpg</t>
+          <t>Celebs/34_Neil_Patrick_Harris_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxdfdfadcfeabjpg.jpg</t>
+          <t>Celebs/34_Neil_Patrick_Harris_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxedaedabcbefbcbabbjpg.jpg</t>
+          <t>Celebs/35_Neil_Patrick_Harris_0009.jpg</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxededbebccdajpg.jpg</t>
+          <t>Celebs/36_Jim_Parsons_0011.jpg</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxeebdfdbaaajpg.jpg</t>
+          <t>Celebs/36_Neil_Patrick_Harris_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxeedccadejpg.jpg</t>
+          <t>Celebs/36_Neil_Patrick_Harris_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxeeedcacddeccccacfjpg.jpg</t>
+          <t>Celebs/37_Neil_Patrick_Harris_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxfcfcbaeaeddabbjpg.jpg</t>
+          <t>Celebs/37_Neil_Patrick_Harris_0014.jpg</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxfecfecaefaadfebejpg.jpg</t>
+          <t>Celebs/37_Will_Smith_0015.jpg</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxfeebfdccajpg.jpg</t>
+          <t>Celebs/38_Jim_Parsons_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxfefdacfbfdeadajpg.jpg</t>
+          <t>Celebs/38_Neil_Patrick_Harris_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxffabffabbbcfbceaedjpg.jpg</t>
+          <t>Celebs/38_Will_Smith_0013.jpg</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxffeabacaaejpg.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0001.jpg</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Dataset/httpssmediacacheakpinimgcomxffecfafddjpg.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Dataset/httpssvagalumecommadonnaimagesmadonnajpg.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Dataset/httpstatictherichestimagescomcdncwpcontentuploadsJerrySeinfeldjpg.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Dataset/httpsticketmnettmenusdamabbacdaebeafdbbCUSTOMjpg.jpg</t>
+          <t>Celebs/39_Neil_Patrick_Harris_0001.jpg</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Dataset/httpsticketmnettmenusdbimagesajpg.jpg</t>
+          <t>Celebs/39_Neil_Patrick_Harris_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Dataset/httpsuploadwikimediaorgwikipediacommonsMadonnathAnnualGoldenGlobesAwardscroppedjpg.jpg</t>
+          <t>Celebs/40_Jim_Parsons_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Dataset/httpsuploadwikimediaorgwikipediacommonsthumbaaMadonnaatthepremiereofIAmBecauseWeArejpgpxMadonnaatthepremiereofIAmBecauseWeArejpg.jpg</t>
+          <t>Celebs/40_Jim_Parsons_0015.jpg</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Dataset/httpsuploadwikimediaorgwikipediacommonsthumbbJerrySeinfeldjpgpxJerrySeinfeldjpg.jpg</t>
+          <t>Celebs/40_Will_Smith_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Dataset/httpsuploadwikimediaorgwikipediacommonsthumbddBenAffleckbyGageSkidmorejpgpxBenAffleckbyGageSkidmorejpg.jpg</t>
+          <t>Celebs/42_Will_Smith_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Dataset/httpsuploadwikimediaorgwikipediacommonsthumbEltonJohninsjpgpxEltonJohninsjpg.jpg</t>
+          <t>Celebs/43_Will_Smith_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Dataset/httpsuploadwikimediaorgwikipediacommonsthumbMindyBKalingBPaleyFestBNewBYorkBBMindyBIqZgUWvbljpgpxMindyBKalingBPaleyFestBNewBYorkBBMindyBIqZgUWvbljpg.jpg</t>
+          <t>Celebs/43_Will_Smith_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Dataset/httpsuswestamazonawscomblogsprodmediausuploadsJerrySeinfeldkidsxjpg.jpg</t>
+          <t>Celebs/43_Will_Smith_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Dataset/httpswwwticketscomuploadsartistsjerryseinfeldbilletsjpg.jpg</t>
+          <t>Celebs/44_Will_Smith_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Dataset/httptrwebimgacstanetcxbdddmediasnmediajpg.jpg</t>
+          <t>Celebs/44_Will_Smith_0007.jpg</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Dataset/httpuploadwikimediaorgwikipediacommonsthumbaMadonnaRotterdamjpgpxMadonnaRotterdamjpg.jpg</t>
+          <t>Celebs/44_Will_Smith_0015.jpg</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwaceshowbizcomimagesphotobenaffleckjpg.jpg</t>
+          <t>Celebs/45_Johnny_Depp_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwadweekcomfilesimagecachenodeinlinemindykalingprofilehedjpg.jpg</t>
+          <t>Celebs/45_Will_Smith_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwallposterscomimagesPostersPFjpg.jpg</t>
+          <t>Celebs/45_Will_Smith_0014.jpg</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwbeastiemaniacomwhoismadonnamadonnajpg.jpg</t>
+          <t>Celebs/47_Johnny_Depp_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwblackdogfilmscomwordpresswpcontentuploadsmadonnacelebrationxjpg.jpg</t>
+          <t>Celebs/47_Johnny_Depp_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwbooksforbetterlivingcomwpcontentuploadsMindyKalingAuthorPhotojpg.jpg</t>
+          <t>Celebs/47_Johnny_Depp_0009.jpg</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwdeadlinecomvimgnetwpcontentuploadseltonjpg.jpg</t>
+          <t>Celebs/48_Johnny_Depp_0001.jpg</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Dataset/httpwwweonlinecomeolimagesEntireSiteregKalingCancermhjpg.jpg</t>
+          <t>Celebs/48_Johnny_Depp_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Dataset/httpwwweonlinecomresizewwweonlinecomeolimagesEntireSitersxEltonJohnJRjpg.jpg</t>
+          <t>Celebs/48_Johnny_Depp_0005.jpg</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Dataset/httpwwweonlinecomresizewwweonlinecomeolimagesEntireSitersxjerryseinfeldjulialouisdreyfusjwjpg.jpg</t>
+          <t>Celebs/49_Johnny_Depp_0013.jpg</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwetonlinecomphotomadonnabdayjpg.jpg</t>
+          <t>Celebs/50_Jackie_Chan_0012.jpg</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwfilmscoopitcgibinattoriBENAFFLECKBENAFFLECKjpg.jpg</t>
+          <t>Celebs/50_Jackie_Chan_0014.jpg</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwhillsindcomstorebenjpg.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0004.jpg</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwimpropercomimagesuploadsusercontentimagesSoroffMindyjpg.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwjohnpauljonesarenacomeventimagesEltonCalendarVjpg.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwlautdeEltonJohneltonjohnjpg.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0018.jpg</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwnndbcompeoplejerryseinfeldaujpg.jpg</t>
+          <t>Celebs/51_Jackie_Chan_0006.jpg</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwpictureszimbiocomfpMindyKalingfBgaONVFDFmjpg.jpg</t>
+          <t>Celebs/52_Jackie_Chan_0002.jpg</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwpictureszimbiocomgiMindyKalingLkvEhTwDeJmjpg.jpg</t>
+          <t>Celebs/54_Jackie_Chan_0001.jpg</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwpictureszimbiocomgpJerrySeinfeldJessicaSeinfeldmarriedBczSipMdNMQljpg.jpg</t>
+          <t>Celebs/54_Jackie_Chan_0014.jpg</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwpsychiatrictimescomsitesdefaultfilesimagesmediaPTMofficSeinfeldjpg.jpg</t>
+          <t>Celebs/55_Jackie_Chan_0003.jpg</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwrumenewscomwpcontentuploadsbenafflekxpng.jpg</t>
+          <t>Celebs/55_Jackie_Chan_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwslatecomcontentdamslateblogsbrowbeatseinfeldjpgCROParticlemediumjpg.jpg</t>
+          <t>Celebs/55_Jackie_Chan_0015.jpg</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Dataset/httpwwwwatchidcomsitesdefaultfilesuploadsightingBreitlingwatchJerrySeinfeldjpg.jpg</t>
+          <t>Celebs/57_Jackie_Chan_0008.jpg</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>non_target</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Celebs/57_Jackie_Chan_0010.jpg</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>non_target</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Celebs/58_Jackie_Chan_0005.jpg</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>non_target</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Prevenção de 2 targets cosecutivos
</commit_message>
<xml_diff>
--- a/stims.xlsx
+++ b/stims.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Celebs/14_Emma_Watson_0004.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0010.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Celebs/14_Emma_Watson_0005.jpg</t>
+          <t>Celebs/22_Emma_Stone_0013.jpg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Celebs/14_Emma_Watson_0008.jpg</t>
+          <t>Celebs/29_Scarlett_Johansson_0016.jpg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Celebs/14_Emma_Watson_0013.jpg</t>
+          <t>Celebs/58_Jackie_Chan_0005.jpg</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Celebs/14_Emma_Watson_0015.jpg</t>
+          <t>Celebs/39_Neil_Patrick_Harris_0001.jpg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Celebs/15_Margot_Robbie_0005.jpg</t>
+          <t>Celebs/36_Neil_Patrick_Harris_0007.jpg</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,19 +520,19 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Celebs/15_Margot_Robbie_0012.jpg</t>
+          <t>Celebs/23_Daniel_Radcliffe_0019.jpg</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Celebs/16_Emma_Stone_0008.jpg</t>
+          <t>Celebs/54_Jackie_Chan_0001.jpg</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,19 +544,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Celebs/16_Emma_Stone_0010.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0012.jpg</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Celebs/16_Emma_Stone_0012.jpg</t>
+          <t>Celebs/47_Johnny_Depp_0003.jpg</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Celebs/16_Emma_Stone_0014.jpg</t>
+          <t>Celebs/24_Scarlett_Johansson_0001.jpg</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Celebs/16_Margot_Robbie_0009.jpg</t>
+          <t>Celebs/22_Emma_Watson_0010.jpg</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,19 +592,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Celebs/17_Daniel_Radcliffe_0007.jpg</t>
+          <t>Celebs/23_Emma_Stone_0014.jpg</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Celebs/17_Emma_Watson_0006.jpg</t>
+          <t>Celebs/38_Will_Smith_0013.jpg</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Celebs/17_Margot_Robbie_0006.jpg</t>
+          <t>Celebs/14_Emma_Watson_0004.jpg</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,55 +628,55 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Celebs/17_Margot_Robbie_0012.jpg</t>
+          <t>Celebs/23_Daniel_Radcliffe_0010.jpg</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Celebs/17_Margot_Robbie_0014.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0008.jpg</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Celebs/18_Daniel_Radcliffe_0002.jpg</t>
+          <t>Celebs/17_Margot_Robbie_0006.jpg</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Celebs/18_Daniel_Radcliffe_0007.jpg</t>
+          <t>Celebs/22_Margot_Robbie_0010.jpg</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Celebs/18_Daniel_Radcliffe_0008.jpg</t>
+          <t>Celebs/17_Daniel_Radcliffe_0007.jpg</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Celebs/18_Emma_Stone_0016.jpg</t>
+          <t>Celebs/14_Emma_Watson_0013.jpg</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Celebs/18_Emma_Watson_0004.jpg</t>
+          <t>Celebs/21_Emma_Watson_0004.jpg</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Celebs/19_Emma_Stone_0006.jpg</t>
+          <t>Celebs/43_Will_Smith_0010.jpg</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Celebs/19_Margot_Robbie_0001.jpg</t>
+          <t>Celebs/47_Johnny_Depp_0009.jpg</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Celebs/19_Margot_Robbie_0004.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0018.jpg</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Celebs/20_Emma_Stone_0005.jpg</t>
+          <t>Celebs/21_Emma_Stone_0003.jpg</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Celebs/20_Emma_Watson_0007.jpg</t>
+          <t>Celebs/14_Emma_Watson_0005.jpg</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -772,7 +772,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Celebs/20_Margot_Robbie_0004.jpg</t>
+          <t>Celebs/21_Margot_Robbie_0003.jpg</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -784,19 +784,19 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Celebs/20_Margot_Robbie_0006.jpg</t>
+          <t>Celebs/18_Daniel_Radcliffe_0008.jpg</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Celebs/20_Scarlett_Johansson_0011.jpg</t>
+          <t>Celebs/55_Jackie_Chan_0003.jpg</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,55 +808,55 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Celebs/21_Daniel_Radcliffe_0002.jpg</t>
+          <t>Celebs/55_Jackie_Chan_0015.jpg</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Celebs/21_Daniel_Radcliffe_0008.jpg</t>
+          <t>Celebs/38_Neil_Patrick_Harris_0006.jpg</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Celebs/21_Daniel_Radcliffe_0009.jpg</t>
+          <t>Celebs/25_Scarlett_Johansson_0010.jpg</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Celebs/21_Daniel_Radcliffe_0012.jpg</t>
+          <t>Celebs/49_Johnny_Depp_0013.jpg</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Celebs/21_Emma_Stone_0002.jpg</t>
+          <t>Celebs/33_Jim_Parsons_0011.jpg</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Celebs/21_Emma_Stone_0003.jpg</t>
+          <t>Celebs/20_Margot_Robbie_0006.jpg</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Celebs/21_Emma_Watson_0004.jpg</t>
+          <t>Celebs/14_Emma_Watson_0008.jpg</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Celebs/21_Margot_Robbie_0003.jpg</t>
+          <t>Celebs/37_Neil_Patrick_Harris_0014.jpg</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Celebs/21_Scarlett_Johansson_0007.jpg</t>
+          <t>Celebs/50_Jackie_Chan_0014.jpg</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Celebs/22_Emma_Stone_0013.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0004.jpg</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Celebs/22_Emma_Watson_0001.jpg</t>
+          <t>Celebs/16_Emma_Stone_0014.jpg</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -940,7 +940,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Celebs/22_Emma_Watson_0003.jpg</t>
+          <t>Celebs/44_Will_Smith_0006.jpg</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Celebs/22_Emma_Watson_0010.jpg</t>
+          <t>Celebs/19_Margot_Robbie_0004.jpg</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Celebs/22_Margot_Robbie_0010.jpg</t>
+          <t>Celebs/50_Jackie_Chan_0012.jpg</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -988,43 +988,43 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Celebs/23_Daniel_Radcliffe_0002.jpg</t>
+          <t>Celebs/40_Jim_Parsons_0015.jpg</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Celebs/23_Daniel_Radcliffe_0010.jpg</t>
+          <t>Celebs/32_Jim_Parsons_0018.jpg</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Celebs/23_Daniel_Radcliffe_0019.jpg</t>
+          <t>Celebs/26_Scarlett_Johansson_0008.jpg</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Celebs/23_Emma_Stone_0014.jpg</t>
+          <t>Celebs/16_Emma_Stone_0008.jpg</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1036,19 +1036,19 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Celebs/24_Daniel_Radcliffe_0017.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0001.jpg</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>non_target</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Celebs/24_Emma_Stone_0015.jpg</t>
+          <t>Celebs/28_Scarlett_Johansson_0005.jpg</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Celebs/24_Scarlett_Johansson_0001.jpg</t>
+          <t>Celebs/19_Margot_Robbie_0001.jpg</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1072,7 +1072,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Celebs/24_Scarlett_Johansson_0011.jpg</t>
+          <t>Celebs/18_Emma_Stone_0016.jpg</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Celebs/25_Scarlett_Johansson_0010.jpg</t>
+          <t>Celebs/38_Jim_Parsons_0003.jpg</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Celebs/26_Scarlett_Johansson_0003.jpg</t>
+          <t>Celebs/48_Johnny_Depp_0005.jpg</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Celebs/26_Scarlett_Johansson_0008.jpg</t>
+          <t>Celebs/48_Johnny_Depp_0003.jpg</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1120,7 +1120,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Celebs/27_Scarlett_Johansson_0012.jpg</t>
+          <t>Celebs/14_Emma_Watson_0015.jpg</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1132,7 +1132,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Celebs/28_Scarlett_Johansson_0005.jpg</t>
+          <t>Celebs/24_Emma_Stone_0015.jpg</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1144,7 +1144,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Celebs/29_Scarlett_Johansson_0010.jpg</t>
+          <t>Celebs/22_Emma_Watson_0001.jpg</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Celebs/29_Scarlett_Johansson_0016.jpg</t>
+          <t>Celebs/45_Will_Smith_0014.jpg</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1168,19 +1168,19 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Celebs/31_Neil_Patrick_Harris_0008.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0002.jpg</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Celebs/32_Jim_Parsons_0010.jpg</t>
+          <t>Celebs/43_Will_Smith_0006.jpg</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Celebs/32_Jim_Parsons_0016.jpg</t>
+          <t>Celebs/57_Jackie_Chan_0010.jpg</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Celebs/32_Jim_Parsons_0018.jpg</t>
+          <t>Celebs/20_Emma_Stone_0005.jpg</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1216,7 +1216,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Celebs/33_Jim_Parsons_0011.jpg</t>
+          <t>Celebs/42_Will_Smith_0012.jpg</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Celebs/33_Neil_Patrick_Harris_0011.jpg</t>
+          <t>Celebs/44_Will_Smith_0007.jpg</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1240,7 +1240,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Celebs/34_Neil_Patrick_Harris_0004.jpg</t>
+          <t>Celebs/19_Emma_Stone_0006.jpg</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Celebs/34_Neil_Patrick_Harris_0007.jpg</t>
+          <t>Celebs/17_Margot_Robbie_0012.jpg</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1264,7 +1264,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Celebs/35_Neil_Patrick_Harris_0009.jpg</t>
+          <t>Celebs/52_Jackie_Chan_0002.jpg</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1276,7 +1276,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Celebs/36_Jim_Parsons_0011.jpg</t>
+          <t>Celebs/45_Will_Smith_0010.jpg</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1288,7 +1288,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Celebs/36_Neil_Patrick_Harris_0007.jpg</t>
+          <t>Celebs/16_Emma_Stone_0012.jpg</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1300,19 +1300,19 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Celebs/36_Neil_Patrick_Harris_0010.jpg</t>
+          <t>Celebs/24_Daniel_Radcliffe_0017.jpg</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Celebs/37_Neil_Patrick_Harris_0010.jpg</t>
+          <t>Celebs/57_Jackie_Chan_0008.jpg</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Celebs/37_Neil_Patrick_Harris_0014.jpg</t>
+          <t>Celebs/40_Jim_Parsons_0004.jpg</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Celebs/37_Will_Smith_0015.jpg</t>
+          <t>Celebs/43_Will_Smith_0007.jpg</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1348,7 +1348,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Celebs/38_Jim_Parsons_0003.jpg</t>
+          <t>Celebs/18_Emma_Watson_0004.jpg</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1360,7 +1360,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Celebs/38_Neil_Patrick_Harris_0006.jpg</t>
+          <t>Celebs/47_Johnny_Depp_0004.jpg</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1372,19 +1372,19 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Celebs/38_Will_Smith_0013.jpg</t>
+          <t>Celebs/23_Daniel_Radcliffe_0002.jpg</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Celebs/39_Jim_Parsons_0001.jpg</t>
+          <t>Celebs/27_Scarlett_Johansson_0012.jpg</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1396,7 +1396,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Celebs/39_Jim_Parsons_0004.jpg</t>
+          <t>Celebs/36_Neil_Patrick_Harris_0010.jpg</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1408,7 +1408,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Celebs/39_Jim_Parsons_0008.jpg</t>
+          <t>Celebs/15_Margot_Robbie_0005.jpg</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1420,19 +1420,19 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Celebs/39_Jim_Parsons_0010.jpg</t>
+          <t>Celebs/18_Daniel_Radcliffe_0007.jpg</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Celebs/39_Neil_Patrick_Harris_0001.jpg</t>
+          <t>Celebs/15_Margot_Robbie_0012.jpg</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1444,19 +1444,19 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Celebs/39_Neil_Patrick_Harris_0010.jpg</t>
+          <t>Celebs/21_Daniel_Radcliffe_0009.jpg</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Celebs/40_Jim_Parsons_0004.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0008.jpg</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1468,7 +1468,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Celebs/40_Jim_Parsons_0015.jpg</t>
+          <t>Celebs/29_Scarlett_Johansson_0010.jpg</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Celebs/40_Will_Smith_0012.jpg</t>
+          <t>Celebs/36_Jim_Parsons_0011.jpg</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Celebs/42_Will_Smith_0012.jpg</t>
+          <t>Celebs/35_Neil_Patrick_Harris_0009.jpg</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Celebs/43_Will_Smith_0006.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0004.jpg</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Celebs/43_Will_Smith_0007.jpg</t>
+          <t>Celebs/39_Jim_Parsons_0008.jpg</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1528,7 +1528,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Celebs/43_Will_Smith_0010.jpg</t>
+          <t>Celebs/17_Emma_Watson_0006.jpg</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Celebs/44_Will_Smith_0006.jpg</t>
+          <t>Celebs/22_Emma_Watson_0003.jpg</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Celebs/44_Will_Smith_0007.jpg</t>
+          <t>Celebs/55_Jackie_Chan_0008.jpg</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1564,7 +1564,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Celebs/44_Will_Smith_0015.jpg</t>
+          <t>Celebs/37_Neil_Patrick_Harris_0010.jpg</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Celebs/45_Johnny_Depp_0003.jpg</t>
+          <t>Celebs/39_Neil_Patrick_Harris_0010.jpg</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Celebs/45_Will_Smith_0010.jpg</t>
+          <t>Celebs/16_Emma_Stone_0010.jpg</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1600,7 +1600,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Celebs/45_Will_Smith_0014.jpg</t>
+          <t>Celebs/20_Emma_Watson_0007.jpg</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1612,7 +1612,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Celebs/47_Johnny_Depp_0003.jpg</t>
+          <t>Celebs/51_Jackie_Chan_0006.jpg</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Celebs/47_Johnny_Depp_0004.jpg</t>
+          <t>Celebs/32_Jim_Parsons_0010.jpg</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Celebs/47_Johnny_Depp_0009.jpg</t>
+          <t>Celebs/31_Neil_Patrick_Harris_0008.jpg</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1648,7 +1648,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Celebs/48_Johnny_Depp_0001.jpg</t>
+          <t>Celebs/24_Scarlett_Johansson_0011.jpg</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Celebs/48_Johnny_Depp_0003.jpg</t>
+          <t>Celebs/44_Will_Smith_0015.jpg</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Celebs/48_Johnny_Depp_0005.jpg</t>
+          <t>Celebs/32_Jim_Parsons_0016.jpg</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1684,7 +1684,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Celebs/49_Johnny_Depp_0013.jpg</t>
+          <t>Celebs/21_Emma_Stone_0002.jpg</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1696,7 +1696,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Celebs/50_Jackie_Chan_0012.jpg</t>
+          <t>Celebs/34_Neil_Patrick_Harris_0004.jpg</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1708,7 +1708,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Celebs/50_Jackie_Chan_0014.jpg</t>
+          <t>Celebs/26_Scarlett_Johansson_0003.jpg</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1720,7 +1720,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Celebs/50_Johnny_Depp_0004.jpg</t>
+          <t>Celebs/48_Johnny_Depp_0001.jpg</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1732,7 +1732,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Celebs/50_Johnny_Depp_0008.jpg</t>
+          <t>Celebs/16_Margot_Robbie_0009.jpg</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1744,7 +1744,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Celebs/50_Johnny_Depp_0010.jpg</t>
+          <t>Celebs/45_Johnny_Depp_0003.jpg</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Celebs/50_Johnny_Depp_0018.jpg</t>
+          <t>Celebs/20_Scarlett_Johansson_0011.jpg</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1768,7 +1768,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Celebs/51_Jackie_Chan_0006.jpg</t>
+          <t>Celebs/40_Will_Smith_0012.jpg</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1780,7 +1780,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Celebs/52_Jackie_Chan_0002.jpg</t>
+          <t>Celebs/54_Jackie_Chan_0014.jpg</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1792,7 +1792,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Celebs/54_Jackie_Chan_0001.jpg</t>
+          <t>Celebs/33_Neil_Patrick_Harris_0011.jpg</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1804,7 +1804,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Celebs/54_Jackie_Chan_0014.jpg</t>
+          <t>Celebs/37_Will_Smith_0015.jpg</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -1816,7 +1816,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Celebs/55_Jackie_Chan_0003.jpg</t>
+          <t>Celebs/17_Margot_Robbie_0014.jpg</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -1828,7 +1828,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Celebs/55_Jackie_Chan_0008.jpg</t>
+          <t>Celebs/50_Johnny_Depp_0010.jpg</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Celebs/55_Jackie_Chan_0015.jpg</t>
+          <t>Celebs/20_Margot_Robbie_0004.jpg</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -1852,7 +1852,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Celebs/57_Jackie_Chan_0008.jpg</t>
+          <t>Celebs/34_Neil_Patrick_Harris_0007.jpg</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1864,7 +1864,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Celebs/57_Jackie_Chan_0010.jpg</t>
+          <t>Celebs/21_Scarlett_Johansson_0007.jpg</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1876,12 +1876,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Celebs/58_Jackie_Chan_0005.jpg</t>
+          <t>Celebs/18_Daniel_Radcliffe_0002.jpg</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>non_target</t>
+          <t>target</t>
         </is>
       </c>
     </row>

</xml_diff>